<commit_message>
Add test kohde without any osapuoli
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_update.xlsx
+++ b/tests/data/test_data_import/DVV_update.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="R1 rakennus" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="152">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -168,6 +168,15 @@
   </si>
   <si>
     <t xml:space="preserve">398</t>
+  </si>
+  <si>
+    <t xml:space="preserve">145678901C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39800300010001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salattu</t>
   </si>
   <si>
     <t xml:space="preserve">Osoite-numero</t>
@@ -721,10 +730,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1135,6 +1144,71 @@
       </c>
       <c r="Y6" s="2" t="n">
         <v>428759</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>20210101</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>260</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T7" s="2" t="n">
+        <v>20210101</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X7" s="2" t="n">
+        <v>6762345</v>
+      </c>
+      <c r="Y7" s="2" t="n">
+        <v>431007</v>
+      </c>
+      <c r="Z7" s="2" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1153,10 +1227,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1174,25 +1248,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,10 +1280,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
@@ -1218,10 +1292,10 @@
         <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1235,7 +1309,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="n">
@@ -1245,10 +1319,10 @@
         <v>35</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>44</v>
@@ -1271,10 +1345,10 @@
         <v>15100</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1288,19 +1362,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,7 +1388,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>9</v>
@@ -1323,10 +1397,36 @@
         <v>35</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1366,70 +1466,70 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,7 +1540,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D2" s="9"/>
       <c r="F2" s="9" t="n">
@@ -1450,37 +1550,37 @@
         <v>1</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>444</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>20100101</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1491,7 +1591,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D3" s="9"/>
       <c r="F3" s="9" t="n">
@@ -1501,25 +1601,25 @@
         <v>1</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>20220101</v>
@@ -1535,7 +1635,7 @@
         <v>398</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>20100101</v>
@@ -1547,16 +1647,16 @@
         <v>30</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,7 +1667,7 @@
         <v>560</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>19980601</v>
@@ -1576,25 +1676,25 @@
         <v>1</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="N5" s="1" t="n">
         <v>16200</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="P5" s="2" t="n">
         <v>19860101</v>
@@ -1608,7 +1708,7 @@
         <v>398</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>20010601</v>
@@ -1617,16 +1717,16 @@
         <v>1</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1647,7 +1747,7 @@
   </sheetPr>
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1667,43 +1767,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,34 +1814,34 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="K2" s="8" t="n">
         <v>15230</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>20220101</v>
@@ -1764,31 +1864,31 @@
         <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M3" s="9" t="n">
         <v>20200101</v>
@@ -1811,31 +1911,31 @@
         <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M4" s="9" t="n">
         <v>20210101</v>
@@ -1855,34 +1955,34 @@
         <v>398</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F5" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M5" s="9" t="n">
         <v>20220101</v>
@@ -1902,34 +2002,34 @@
         <v>398</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F6" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M6" s="9" t="n">
         <v>20220601</v>
@@ -1949,34 +2049,34 @@
         <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="M7" s="2" t="n">
         <v>19860101</v>
@@ -1996,34 +2096,34 @@
         <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M8" s="2" t="n">
         <v>20230201</v>

</xml_diff>

<commit_message>
Set starting and ending dates for kohteet according to changes in owners or habitants
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_update.xlsx
+++ b/tests/data/test_data_import/DVV_update.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="R1 rakennus" sheetId="1" state="visible" r:id="rId2"/>
@@ -732,7 +732,7 @@
   </sheetPr>
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1747,8 +1747,8 @@
   </sheetPr>
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M9" activeCellId="0" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2126,7 +2126,7 @@
         <v>62</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>20230201</v>
+        <v>20230117</v>
       </c>
       <c r="N8" s="2" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Fixed currently fixable tests, leftovers should be fixed during development
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_update.xlsx
+++ b/tests/data/test_data_import/DVV_update.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="R1 rakennus" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="164">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -419,9 +419,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tilapäisten asukk lukumäärä</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rakennus-Luokka</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -531,7 +528,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -558,6 +555,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -620,7 +622,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -705,6 +707,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,11 +790,11 @@
   </sheetPr>
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA28" activeCellId="0" sqref="AA28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="22.95"/>
@@ -1409,10 +1415,10 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.08"/>
@@ -1682,7 +1688,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="34.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="22.95"/>
@@ -2034,13 +2040,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="23.22"/>
@@ -2094,9 +2100,7 @@
       <c r="O1" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="P1" s="19" t="s">
-        <v>131</v>
-      </c>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
@@ -2106,13 +2110,13 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
@@ -2121,10 +2125,10 @@
         <v>105</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>134</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>135</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>108</v>
@@ -2144,9 +2148,7 @@
       <c r="O2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P2" s="20" t="n">
-        <v>1</v>
-      </c>
+      <c r="P2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
@@ -2159,25 +2161,25 @@
         <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>139</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>140</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
@@ -2194,9 +2196,7 @@
       <c r="O3" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="P3" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
@@ -2209,25 +2209,25 @@
         <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>144</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>145</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
@@ -2244,9 +2244,7 @@
       <c r="O4" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="P4" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
@@ -2256,28 +2254,28 @@
         <v>398</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>151</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
@@ -2294,9 +2292,7 @@
       <c r="O5" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="P5" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
@@ -2306,28 +2302,28 @@
         <v>398</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="I6" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="J6" s="10" t="s">
         <v>155</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>156</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>15100</v>
@@ -2344,9 +2340,7 @@
       <c r="O6" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="P6" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
@@ -2356,13 +2350,13 @@
         <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>1</v>
@@ -2371,10 +2365,10 @@
         <v>113</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>115</v>
@@ -2394,9 +2388,7 @@
       <c r="O7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P7" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
@@ -2406,28 +2398,28 @@
         <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>36</v>
@@ -2444,9 +2436,7 @@
       <c r="O8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P8" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
@@ -2456,7 +2446,7 @@
         <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>1</v>
@@ -2465,13 +2455,13 @@
         <v>120</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>36</v>
@@ -2488,9 +2478,14 @@
       <c r="O9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P9" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
+      <c r="D10" s="1"/>
+      <c r="G10" s="2"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fixed test expected end date and counts
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_update.xlsx
+++ b/tests/data/test_data_import/DVV_update.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="R1 rakennus" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="168">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -201,9 +201,6 @@
     <t xml:space="preserve">39800200030003</t>
   </si>
   <si>
-    <t xml:space="preserve">200000002D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Osoite-numero</t>
   </si>
   <si>
@@ -407,12 +404,6 @@
   </si>
   <si>
     <t xml:space="preserve">Lauko Puolikuoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">151046-9874</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kauko Täysikuoma</t>
   </si>
   <si>
     <t xml:space="preserve">Huo-neisto-kirjain</t>
@@ -802,11 +793,11 @@
   </sheetPr>
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ10" activeCellId="0" sqref="AJ10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="22.95"/>
@@ -1471,66 +1462,24 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>19750111</v>
-      </c>
-      <c r="L11" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N11" s="2" t="n">
-        <v>80</v>
-      </c>
-      <c r="O11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="2" t="n">
-        <v>250</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T11" s="2" t="n">
-        <v>19780101</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="V11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="W11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="X11" s="2" t="n">
-        <v>6765334</v>
-      </c>
-      <c r="Y11" s="2" t="n">
-        <v>428759</v>
-      </c>
+      <c r="A11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="8"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1551,10 +1500,10 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.08"/>
@@ -1569,25 +1518,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,10 +1550,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
@@ -1613,10 +1562,10 @@
         <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="n">
@@ -1640,10 +1589,10 @@
         <v>36</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1657,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="10" t="n">
         <v>44</v>
@@ -1666,10 +1615,10 @@
         <v>15100</v>
       </c>
       <c r="H4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1683,19 +1632,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>44</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1709,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>9</v>
@@ -1718,10 +1667,10 @@
         <v>36</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1735,7 +1684,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>99</v>
@@ -1744,10 +1693,10 @@
         <v>36</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1761,7 +1710,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>11</v>
@@ -1770,10 +1719,10 @@
         <v>36</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1787,7 +1736,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>13</v>
@@ -1796,10 +1745,10 @@
         <v>36</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,7 +1762,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>14</v>
@@ -1822,37 +1771,18 @@
         <v>36</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="A11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1872,11 +1802,11 @@
   </sheetPr>
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="34.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="22.95"/>
@@ -1891,70 +1821,70 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1965,7 +1895,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="10"/>
       <c r="F2" s="10" t="n">
@@ -1975,37 +1905,37 @@
         <v>1</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>101</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>444</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>20100101</v>
       </c>
       <c r="Q2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="S2" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,7 +1946,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="10"/>
       <c r="F3" s="10" t="n">
@@ -2026,25 +1956,25 @@
         <v>1</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>36</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>20220101</v>
@@ -2060,7 +1990,7 @@
         <v>398</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F4" s="10" t="n">
         <v>20100101</v>
@@ -2072,16 +2002,16 @@
         <v>31</v>
       </c>
       <c r="I4" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q4" s="10" t="s">
         <v>113</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>114</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2092,7 +2022,7 @@
         <v>560</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>19980601</v>
@@ -2101,25 +2031,25 @@
         <v>1</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N5" s="1" t="n">
         <v>16200</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P5" s="2" t="n">
         <v>19860101</v>
@@ -2133,7 +2063,7 @@
         <v>398</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>20010601</v>
@@ -2142,16 +2072,16 @@
         <v>1</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2162,7 +2092,7 @@
         <v>398</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>20230123</v>
@@ -2171,16 +2101,16 @@
         <v>1</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2191,7 +2121,7 @@
         <v>398</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>20010601</v>
@@ -2200,16 +2130,16 @@
         <v>1</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J8" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2220,7 +2150,7 @@
         <v>560</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>20250101</v>
@@ -2229,70 +2159,43 @@
         <v>1</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N9" s="1" t="n">
         <v>16200</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P9" s="2" t="n">
         <v>19860101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>560</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>20250101</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="N10" s="1" t="n">
-        <v>16200</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="P10" s="2" t="n">
-        <v>19860101</v>
-      </c>
+      <c r="A10" s="8"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="9"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2312,11 +2215,11 @@
   </sheetPr>
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="23.22"/>
@@ -2332,43 +2235,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="I1" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="16" t="s">
+      <c r="J1" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="K1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="O1" s="18" t="s">
         <v>134</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>137</v>
       </c>
       <c r="P1" s="19"/>
     </row>
@@ -2380,34 +2283,34 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>141</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K2" s="9" t="n">
         <v>15230</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>20220101</v>
@@ -2431,31 +2334,31 @@
         <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>143</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>146</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M3" s="10" t="n">
         <v>20200101</v>
@@ -2479,31 +2382,31 @@
         <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>148</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>151</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M4" s="10" t="n">
         <v>20210101</v>
@@ -2524,34 +2427,34 @@
         <v>398</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="I5" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>154</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>157</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M5" s="10" t="n">
         <v>20220101</v>
@@ -2572,34 +2475,34 @@
         <v>398</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="J6" s="10" t="s">
         <v>159</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>162</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M6" s="10" t="n">
         <v>20220601</v>
@@ -2620,34 +2523,34 @@
         <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M7" s="2" t="n">
         <v>19860101</v>
@@ -2668,34 +2571,34 @@
         <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>36</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M8" s="2" t="n">
         <v>20220617</v>
@@ -2716,28 +2619,28 @@
         <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>36</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M9" s="2" t="n">
         <v>20010603</v>

</xml_diff>

<commit_message>
Couple of fixes to allow assertion errors in expected format
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_update.xlsx
+++ b/tests/data/test_data_import/DVV_update.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="R1 rakennus" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="170">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -404,6 +404,12 @@
   </si>
   <si>
     <t xml:space="preserve">Lauko Puolikuoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">151046-9880</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyykoski Joseph</t>
   </si>
   <si>
     <t xml:space="preserve">Huo-neisto-kirjain</t>
@@ -793,11 +799,11 @@
   </sheetPr>
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AJ10" activeCellId="0" sqref="AJ10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="22.95"/>
@@ -1503,7 +1509,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.08"/>
@@ -1802,11 +1808,11 @@
   </sheetPr>
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="34.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="22.95"/>
@@ -2184,18 +2190,45 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="9"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="A10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>560</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>20250101</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <v>16200</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P10" s="2" t="n">
+        <v>19860101</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2219,7 +2252,7 @@
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="23.22"/>
@@ -2235,28 +2268,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>58</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>87</v>
@@ -2268,10 +2301,10 @@
         <v>89</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P1" s="19"/>
     </row>
@@ -2283,13 +2316,13 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
@@ -2298,10 +2331,10 @@
         <v>107</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>110</v>
@@ -2334,25 +2367,25 @@
         <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F3" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
@@ -2382,25 +2415,25 @@
         <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F4" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
@@ -2427,28 +2460,28 @@
         <v>398</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F5" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
@@ -2475,28 +2508,28 @@
         <v>398</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F6" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>15100</v>
@@ -2523,13 +2556,13 @@
         <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>1</v>
@@ -2538,10 +2571,10 @@
         <v>115</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>117</v>
@@ -2571,28 +2604,28 @@
         <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>36</v>
@@ -2619,7 +2652,7 @@
         <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>1</v>
@@ -2628,13 +2661,13 @@
         <v>122</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>36</v>

</xml_diff>